<commit_message>
það skarast áfangar en ég get ekki lagað það
</commit_message>
<xml_diff>
--- a/stundatafla.xlsx
+++ b/stundatafla.xlsx
@@ -633,10 +633,14 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (landsbyggd)</t>
@@ -658,7 +662,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -715,10 +723,14 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (landsbyggd)</t>
@@ -740,7 +752,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
@@ -792,7 +808,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (landsbyggd)</t>
@@ -814,7 +834,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
@@ -870,7 +894,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (landsbyggd)</t>
@@ -892,7 +920,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -941,10 +973,14 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -966,7 +1002,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -1015,10 +1055,14 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1040,7 +1084,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -1089,10 +1137,14 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1114,7 +1166,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -1147,10 +1203,14 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1172,7 +1232,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1243,7 +1307,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
@@ -1294,7 +1362,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1317,7 +1389,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
@@ -1368,7 +1444,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1391,7 +1471,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
@@ -1431,10 +1515,14 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1457,7 +1545,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
@@ -1513,10 +1605,14 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1539,7 +1635,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
@@ -1587,10 +1687,14 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1613,7 +1717,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
@@ -1687,7 +1795,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
@@ -1723,10 +1835,14 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>Heimahjúkrun HJÚ711G (hofudborgarsvaedi)</t>
@@ -1749,7 +1865,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
@@ -1805,10 +1925,14 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -1839,7 +1963,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="X18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
@@ -1871,10 +1999,14 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -1905,7 +2037,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="X19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
@@ -1953,10 +2089,14 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -1989,7 +2129,7 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2027,10 +2167,14 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
@@ -2063,7 +2207,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2101,10 +2245,14 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -2137,7 +2285,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr"/>
@@ -2199,7 +2347,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="Z23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
@@ -2221,10 +2373,14 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
@@ -2253,7 +2409,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>Líknarmeðferð HJÚ0AXM (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Líknarmeðferð HJÚ0AXM (val)</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr"/>
@@ -2299,10 +2455,14 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
@@ -2340,7 +2500,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AA25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AB25" t="inlineStr">
         <is>
           <t>Kynheilbrigði HJÚ823M (val)</t>
@@ -2381,10 +2545,14 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
@@ -2434,7 +2602,7 @@
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AD26" t="inlineStr">
@@ -2466,7 +2634,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
@@ -2500,7 +2672,7 @@
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
@@ -2548,7 +2720,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
@@ -2581,7 +2757,7 @@
       </c>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2603,10 +2779,14 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðaöldrunarlækningadeild B4 Fossvogi)</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
@@ -2636,7 +2816,7 @@
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
@@ -2681,10 +2861,14 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
@@ -2718,7 +2902,7 @@
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr"/>
@@ -2763,10 +2947,14 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -2797,7 +2985,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="X31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr">
         <is>
@@ -2837,10 +3029,14 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
@@ -2874,7 +3070,7 @@
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
@@ -2919,10 +3115,14 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
@@ -2973,7 +3173,7 @@
       </c>
       <c r="AD33" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AE33" t="inlineStr">
@@ -3001,10 +3201,14 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
@@ -3031,7 +3235,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="X34" t="inlineStr"/>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Y34" t="inlineStr">
         <is>
           <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
@@ -3079,10 +3287,14 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
@@ -3123,7 +3335,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AD35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
@@ -3145,10 +3361,14 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
@@ -3197,7 +3417,7 @@
       </c>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3233,10 +3453,14 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -3264,7 +3488,7 @@
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="AD37" t="inlineStr"/>
@@ -3291,10 +3515,14 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -3334,7 +3562,7 @@
       </c>
       <c r="AC38" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AD38" t="inlineStr">
@@ -3376,7 +3604,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -3408,7 +3640,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AA39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AB39" t="inlineStr">
         <is>
           <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
@@ -3450,7 +3686,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Heila-, tauga- og bæklunarskurðdeild, B6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -3499,7 +3739,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AF40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="inlineStr"/>
       <c r="AI40" t="inlineStr"/>
@@ -3521,10 +3765,14 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -3558,7 +3806,7 @@
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AB41" t="inlineStr"/>
@@ -3599,10 +3847,14 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
@@ -3635,7 +3887,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AF42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AG42" t="inlineStr"/>
       <c r="AH42" t="inlineStr"/>
       <c r="AI42" t="inlineStr"/>
@@ -3657,10 +3913,14 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
@@ -3693,7 +3953,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr"/>
@@ -3731,10 +3991,14 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
@@ -3777,7 +4041,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AD44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" t="inlineStr">
         <is>
@@ -3808,7 +4076,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -3834,7 +4106,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="Y45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Z45" t="inlineStr">
         <is>
           <t>Kynheilbrigði HJÚ823M (val)</t>
@@ -3890,7 +4166,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
@@ -3919,7 +4199,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr"/>
@@ -3957,10 +4237,14 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
@@ -3989,7 +4273,7 @@
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
@@ -4031,10 +4315,14 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
@@ -4079,7 +4367,7 @@
       </c>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr">
@@ -4113,10 +4401,14 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
@@ -4149,7 +4441,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr"/>
@@ -4183,10 +4475,14 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
@@ -4221,7 +4517,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AD50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
       <c r="AG50" t="inlineStr"/>
@@ -4241,10 +4541,14 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
@@ -4287,7 +4591,7 @@
       </c>
       <c r="AB51" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AC51" t="inlineStr">
@@ -4327,10 +4631,14 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
@@ -4361,7 +4669,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AD52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AE52" t="inlineStr"/>
       <c r="AF52" t="inlineStr">
         <is>
@@ -4385,10 +4697,14 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
@@ -4422,7 +4738,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AC53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AD53" t="inlineStr"/>
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr"/>
@@ -4443,10 +4763,14 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr">
         <is>
@@ -4505,7 +4829,7 @@
       </c>
       <c r="AF54" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AG54" t="inlineStr"/>
@@ -4525,10 +4849,14 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
@@ -4559,7 +4887,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AD55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AE55" t="inlineStr"/>
       <c r="AF55" t="inlineStr"/>
       <c r="AG55" t="inlineStr"/>
@@ -4579,10 +4911,14 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr">
         <is>
@@ -4621,7 +4957,7 @@
       </c>
       <c r="AB56" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AC56" t="inlineStr">
@@ -4709,7 +5045,7 @@
       </c>
       <c r="AD57" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AE57" t="inlineStr">
@@ -4735,10 +5071,14 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
@@ -4797,7 +5137,7 @@
       </c>
       <c r="AF58" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AG58" t="inlineStr"/>
@@ -4817,10 +5157,14 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr">
         <is>
@@ -4879,7 +5223,7 @@
       </c>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AG59" t="inlineStr"/>
@@ -4902,7 +5246,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
@@ -4936,7 +5284,7 @@
       </c>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AB60" t="inlineStr">
@@ -4984,7 +5332,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (HNE-, lýta- og æðaskurðdeild, A4 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
@@ -5043,7 +5395,7 @@
       </c>
       <c r="AF61" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AG61" t="inlineStr"/>
@@ -5063,10 +5415,14 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðaöldrunarlækningadeild B4 Fossvogi)</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
@@ -5105,7 +5461,7 @@
       </c>
       <c r="AB62" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AC62" t="inlineStr">
@@ -5145,10 +5501,14 @@
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Kvenlækningadeild 21A, Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
@@ -5191,7 +5551,7 @@
       </c>
       <c r="AB63" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="AC63" t="inlineStr">
@@ -5227,10 +5587,14 @@
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
@@ -5269,7 +5633,7 @@
       </c>
       <c r="AB64" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AC64" t="inlineStr">
@@ -5305,10 +5669,14 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
@@ -5338,7 +5706,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="Y65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Z65" t="inlineStr"/>
       <c r="AA65" t="inlineStr">
         <is>
@@ -5375,10 +5747,14 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
@@ -5411,7 +5787,7 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr"/>
@@ -5449,10 +5825,14 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
+        </is>
+      </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
@@ -5480,7 +5860,7 @@
       </c>
       <c r="Y67" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="Z67" t="inlineStr"/>
@@ -5535,10 +5915,14 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjarta- og lungnaskurðdeild, og legudeild augndeildar, 12G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
@@ -5572,7 +5956,7 @@
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AB68" t="inlineStr"/>
@@ -5605,10 +5989,14 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
+        </is>
+      </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
@@ -5656,7 +6044,7 @@
       </c>
       <c r="AC69" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AD69" t="inlineStr"/>
@@ -5685,10 +6073,14 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Bæklunarskurðdeild , B5 Fossvogur)</t>
+        </is>
+      </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
@@ -5731,7 +6123,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AB70" t="inlineStr"/>
+      <c r="AB70" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AC70" t="inlineStr">
         <is>
           <t>Kynheilbrigði HJÚ823M (val)</t>
@@ -5771,10 +6167,14 @@
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Taugalækningadeild , B2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Líknardeildin , Líknard. Kópavogi)</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
@@ -5805,7 +6205,7 @@
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AA71" t="inlineStr">
@@ -5841,10 +6241,14 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
@@ -5884,7 +6288,7 @@
       </c>
       <c r="AA72" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AB72" t="inlineStr"/>
@@ -5923,10 +6327,14 @@
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Blóð og krabbameinsdeild, 11EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
@@ -5962,7 +6370,7 @@
       </c>
       <c r="AA73" t="inlineStr">
         <is>
-          <t>Líknarmeðferð HJÚ0AXM (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Líknarmeðferð HJÚ0AXM (val)</t>
         </is>
       </c>
       <c r="AB73" t="inlineStr"/>
@@ -6005,10 +6413,14 @@
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Lungnadeild , A6 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
@@ -6036,7 +6448,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AC74" t="inlineStr"/>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AD74" t="inlineStr"/>
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr"/>
@@ -6062,7 +6478,11 @@
           <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
@@ -6088,7 +6508,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AA75" t="inlineStr"/>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AB75" t="inlineStr"/>
       <c r="AC75" t="inlineStr">
         <is>
@@ -6117,10 +6541,14 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Gigtar og almenn lyflækningadeild , B7 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="I76" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
@@ -6166,7 +6594,7 @@
       </c>
       <c r="AC76" t="inlineStr">
         <is>
-          <t>Kynheilbrigði HJÚ823M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Kynheilbrigði HJÚ823M (val)</t>
         </is>
       </c>
       <c r="AD76" t="inlineStr"/>
@@ -6199,10 +6627,14 @@
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Bráðalyflækningadeild , A2 Fossvogur)</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Endurhæfingardeild, Grensás R2-3)</t>
+        </is>
+      </c>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
@@ -6226,7 +6658,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="Y77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="Z77" t="inlineStr">
         <is>
           <t>Bráðahjúkrun HJÚ824G (brada)</t>
@@ -6281,10 +6717,14 @@
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Þvagfæra- og almenn skurðlækningadeild, 13EG Hringbraut)</t>
+        </is>
+      </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
@@ -6315,7 +6755,7 @@
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>Bráðahjúkrun HJÚ824G (brada)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Bráðahjúkrun HJÚ824G (brada)</t>
         </is>
       </c>
       <c r="AA78" t="inlineStr">
@@ -6363,10 +6803,14 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Smitsjúkdómadeild , A7 Fossvogur)</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
@@ -6423,7 +6867,7 @@
       </c>
       <c r="AF79" t="inlineStr">
         <is>
-          <t>Konur heilsa og samfélag HJÚ827M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Konur heilsa og samfélag HJÚ827M (val)</t>
         </is>
       </c>
       <c r="AG79" t="inlineStr"/>
@@ -6445,10 +6889,14 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
@@ -6492,7 +6940,11 @@
           <t>Barnahjúkrun HJÚ715G (barna)</t>
         </is>
       </c>
-      <c r="AC80" t="inlineStr"/>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>Barnahjúkrun HJÚ715G (barna)</t>
+        </is>
+      </c>
       <c r="AD80" t="inlineStr">
         <is>
           <t>Konur heilsa og samfélag HJÚ827M (val)</t>
@@ -6527,10 +6979,14 @@
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Hjúkrunarstjórnun HJÚ714G (Hjartadeild  , 14 E/G Hringbraut)</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr"/>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Hjúkrunarstjórnun HJÚ714G (Meltingar- og nýrnadeild , 12E Hringbraut)</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
@@ -6575,7 +7031,7 @@
       </c>
       <c r="AF81" t="inlineStr">
         <is>
-          <t>Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
+          <t>Barnahjúkrun HJÚ715G (barna)Andvari: Gjörgæsluhjúkrun HJÚ824M (val)</t>
         </is>
       </c>
       <c r="AG81" t="inlineStr"/>

</xml_diff>